<commit_message>
[New] Basic Frame Work Step 11 (libxl)
- libxl read num test complete.
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\003. Rotem\2021. 01. Vctech_DU_DLL\010_TestProgram_Builder\010_XE7\Source\Win32\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Server\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8FDF6A-3B01-41FA-BD88-F534D2E8319D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8581F29D-F005-44AC-8DA9-AA3C2FF135C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="readme" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -382,11 +383,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898580B5-FCFA-4C27-99D7-BB266403C738}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7099D3B-6E8E-476D-873F-90E8792B81C7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[New] Load Sheet Routine (Step 01)
- Basic Test (Refer to Source)
</commit_message>
<xml_diff>
--- a/Win32/Debug/Config.xlsx
+++ b/Win32/Debug/Config.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wave\010_Project\020_Util\Simulator\Server\010_Source\Win32\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8581F29D-F005-44AC-8DA9-AA3C2FF135C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B8F64D-ACFD-41D4-8217-8B0A9D057061}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,6 +24,51 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44,20 +90,47 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -66,9 +139,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7099D3B-6E8E-476D-873F-90E8792B81C7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -414,4 +502,522 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA55F303-B8EC-432B-8E88-A3126BA97215}">
+  <dimension ref="C6:L38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.625" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="10.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>7</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="5">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
+        <v>8</v>
+      </c>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="5">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="5">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="5">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="5">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="5">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="5">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="5">
+        <v>20</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="5">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="5">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="5">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="5">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="5">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="5">
+        <v>26</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="5">
+        <v>27</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="5">
+        <v>28</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="5">
+        <v>29</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="5">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="5">
+        <v>31</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>